<commit_message>
Actualización del cronograma de tareas
</commit_message>
<xml_diff>
--- a/Cronograma_TFG.xlsx
+++ b/Cronograma_TFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\TFG_Julia\Trabajo_Fin_Grado_GIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312A1A30-1AF2-43FC-A44A-9B346DE324B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06641605-6BA4-41FC-8722-D34FD530B172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>17-23</t>
   </si>
@@ -120,9 +120,6 @@
     <t xml:space="preserve">Adaptación de los parámetros </t>
   </si>
   <si>
-    <t xml:space="preserve">Generación del modelo </t>
-  </si>
-  <si>
     <t>Optimización del modelo</t>
   </si>
   <si>
@@ -139,13 +136,22 @@
   </si>
   <si>
     <t>18-21</t>
+  </si>
+  <si>
+    <t>Integración del sensor al diseño inicial</t>
+  </si>
+  <si>
+    <t>Integración de las bobinas al diseño con sensor</t>
+  </si>
+  <si>
+    <t>Diseño de las capas/estructura del sensor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,8 +195,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3700C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +276,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3700C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -650,11 +669,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -718,6 +752,36 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -745,40 +809,14 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,6 +825,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3700C0"/>
       <color rgb="FFCC0099"/>
       <color rgb="FFEAF4E4"/>
       <color rgb="FF8CBDFE"/>
@@ -795,7 +834,6 @@
       <color rgb="FF215EE7"/>
       <color rgb="FFBFD8EF"/>
       <color rgb="FFAFCEEB"/>
-      <color rgb="FF3700C0"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1072,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,29 +1128,29 @@
     </row>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40" t="s">
+      <c r="D4" s="49"/>
+      <c r="E4" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43" t="s">
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="37" t="s">
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="39"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="49"/>
       <c r="R4" s="10" t="s">
         <v>9</v>
       </c>
@@ -1125,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>11</v>
@@ -1174,7 +1212,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="41" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -1188,7 +1226,7 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="21" t="s">
         <v>23</v>
       </c>
@@ -1200,7 +1238,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="22" t="s">
         <v>25</v>
       </c>
@@ -1212,7 +1250,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="53"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="23" t="s">
         <v>24</v>
       </c>
@@ -1224,7 +1262,7 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="44" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -1238,7 +1276,7 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="24" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1288,7 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="41" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -1264,66 +1302,68 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="52"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="42"/>
+      <c r="B14" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="42"/>
+      <c r="B15" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="60"/>
+    </row>
+    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="43"/>
+      <c r="B16" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="53"/>
-      <c r="B14" s="23" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="56"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="55"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="25"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1331,9 +1371,9 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="47"/>
-      <c r="B19" s="26"/>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="45"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1341,35 +1381,57 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="48"/>
-      <c r="B20" s="5"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="51" t="s">
-        <v>36</v>
-      </c>
+      <c r="A21" s="56"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="50"/>
-      <c r="B22" s="48"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="38"/>
+      <c r="B24" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="E4:H4"/>
     <mergeCell ref="I4:M4"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización cronograma y modelos viabilidad
</commit_message>
<xml_diff>
--- a/Cronograma_TFG.xlsx
+++ b/Cronograma_TFG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\TFG_Julia\Trabajo_Fin_Grado_GIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8881CBE1-7347-4C2A-8530-8F0E08C263B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D120BA10-CFB3-4C58-BA29-224B8A4762CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -897,7 +897,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -959,7 +959,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -982,7 +981,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -990,71 +988,71 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1349,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,30 +1368,30 @@
     </row>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67" t="s">
+      <c r="D4" s="78"/>
+      <c r="E4" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="71" t="s">
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="64" t="s">
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="66"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="78"/>
       <c r="S4" s="7" t="s">
         <v>9</v>
       </c>
@@ -1453,12 +1451,12 @@
       <c r="R5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="S5" s="59" t="s">
+      <c r="S5" s="57" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="68" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -1483,7 +1481,7 @@
       <c r="S6" s="3"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="75"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="17" t="s">
         <v>21</v>
       </c>
@@ -1506,7 +1504,7 @@
       <c r="S7" s="3"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="75"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="18" t="s">
         <v>22</v>
       </c>
@@ -1529,7 +1527,7 @@
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="76"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="19" t="s">
         <v>43</v>
       </c>
@@ -1541,27 +1539,27 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -1577,17 +1575,17 @@
       <c r="S10" s="10"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="78"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1600,21 +1598,21 @@
       <c r="S11" s="3"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="79"/>
-      <c r="B12" s="48" t="s">
+      <c r="A12" s="75"/>
+      <c r="B12" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="47"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="60"/>
+      <c r="M12" s="58"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
@@ -1623,7 +1621,7 @@
       <c r="S12" s="4"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="68" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -1648,7 +1646,7 @@
       <c r="S13" s="10"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="75"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="18" t="s">
         <v>31</v>
       </c>
@@ -1671,7 +1669,7 @@
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="75"/>
+      <c r="A15" s="72"/>
       <c r="B15" s="20" t="s">
         <v>32</v>
       </c>
@@ -1694,7 +1692,7 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="75"/>
+      <c r="A16" s="72"/>
       <c r="B16" s="30" t="s">
         <v>33</v>
       </c>
@@ -1706,7 +1704,7 @@
       <c r="H16" s="28"/>
       <c r="I16" s="36"/>
       <c r="J16" s="36"/>
-      <c r="K16" s="39"/>
+      <c r="K16" s="38"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -1717,20 +1715,20 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="75"/>
+      <c r="A17" s="72"/>
       <c r="B17" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="53"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="52"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -1740,8 +1738,8 @@
       <c r="S17" s="3"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="76"/>
-      <c r="B18" s="48" t="s">
+      <c r="A18" s="69"/>
+      <c r="B18" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="4"/>
@@ -1755,7 +1753,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-      <c r="N18" s="62"/>
+      <c r="N18" s="60"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
@@ -1763,10 +1761,10 @@
       <c r="S18" s="4"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="62" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="10"/>
@@ -1777,9 +1775,9 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="61"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="59"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
@@ -1788,7 +1786,7 @@
       <c r="S19" s="10"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="75"/>
+      <c r="A20" s="72"/>
       <c r="B20" s="30" t="s">
         <v>48</v>
       </c>
@@ -1803,39 +1801,39 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
-      <c r="N20" s="63"/>
-      <c r="O20" s="3"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="61"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="75"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="82"/>
-      <c r="O21" s="84"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="63"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="76"/>
-      <c r="B22" s="48" t="s">
+      <c r="A22" s="69"/>
+      <c r="B22" s="47" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="4"/>
@@ -1849,101 +1847,101 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="83"/>
+      <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
-      <c r="S22" s="3"/>
+      <c r="S22" s="4"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="72" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
       <c r="M23" s="10"/>
-      <c r="N23" s="85"/>
-      <c r="O23" s="86"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="65"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
-      <c r="S23" s="3"/>
+      <c r="S23" s="10"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="75"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="82"/>
-      <c r="O24" s="87"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="66"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="82"/>
-      <c r="O25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="2"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="75"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="82"/>
+      <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -1951,136 +1949,156 @@
       <c r="S26" s="3"/>
     </row>
     <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="76"/>
+      <c r="A27" s="72"/>
       <c r="B27" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="74" t="s">
-        <v>28</v>
-      </c>
+    <row r="28" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="69"/>
       <c r="B28" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
     </row>
     <row r="29" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="80"/>
-      <c r="B29" s="88" t="s">
+      <c r="A29" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" s="74" t="s">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+    </row>
+    <row r="30" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="86"/>
+      <c r="B30" s="70" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="87"/>
+      <c r="N30" s="88"/>
+      <c r="O30" s="88"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+    </row>
+    <row r="31" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="89" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-    </row>
-    <row r="31" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="76"/>
-      <c r="B31" s="90"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="69"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A23:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>